<commit_message>
gn: improve pre stop forms
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Guinea Conakry/gn_oncho_pre_stop_202311_2_participant.xlsx
+++ b/ONCHO/Impact Assessments/Guinea Conakry/gn_oncho_pre_stop_202311_2_participant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Guinea Conakry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7160966A-53C0-4D24-9CB9-2D79389E00DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A03B09D-8D4A-4DED-84E9-07D438D387A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
   <si>
     <t>type</t>
   </si>
@@ -871,7 +871,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6:L7"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1194,7 +1194,9 @@
       <c r="E13" s="31"/>
       <c r="F13" s="32"/>
       <c r="G13" s="33"/>
-      <c r="H13" s="32"/>
+      <c r="H13" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="I13" s="16"/>
       <c r="J13" s="32" t="s">
         <v>15</v>

</xml_diff>